<commit_message>
Mapped out relations for Pokemon, Abilities, and Moves
</commit_message>
<xml_diff>
--- a/DBSchema.xlsx
+++ b/DBSchema.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>Pokemon</t>
   </si>
@@ -25,7 +25,7 @@
     <t>primary_key</t>
   </si>
   <si>
-    <t>num</t>
+    <t>number</t>
   </si>
   <si>
     <t>string</t>
@@ -89,6 +89,81 @@
   </si>
   <si>
     <t>other forms</t>
+  </si>
+  <si>
+    <t>Abilities</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>https://github.com/Zarel/Pokemon-Showdown/blob/master/data/abilities.js</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Short description</t>
+  </si>
+  <si>
+    <t>Moves</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>base_power</t>
+  </si>
+  <si>
+    <t>(Special, Status, physical)</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>short_descrption</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flags </t>
+  </si>
+  <si>
+    <t>protect, mirror, heal, snatch</t>
+  </si>
+  <si>
+    <t>drain</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>chance, boosts</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>isContact</t>
+  </si>
+  <si>
+    <t>isNotProtectable</t>
+  </si>
+  <si>
+    <t>critRatio</t>
   </si>
 </sst>
 </file>
@@ -116,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -124,6 +199,139 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -145,8 +353,41 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -493,148 +734,346 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09016393442623" defaultRowHeight="13.95" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.09016393442623" defaultRowHeight="13.95" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.9426229508197" customWidth="1"/>
-    <col min="2" max="2" width="11.8688524590164" customWidth="1"/>
+    <col min="2" max="2" width="14.655737704918" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" ht="14.7" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>